<commit_message>
Update on Dead-Ends fixing
</commit_message>
<xml_diff>
--- a/Notebooks/temp/mass_unbalanced_reactions.xlsx
+++ b/Notebooks/temp/mass_unbalanced_reactions.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D755"/>
+  <dimension ref="A1:D756"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17043,6 +17043,28 @@
         </is>
       </c>
     </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>XOLESTPOOL</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>xolest_cho_l &lt;=&gt; 0.138 HC02020_l + 0.0001 HC02021_l + 0.0132 HC02022_l + 0.1958 HC02023_l + 0.5254 HC02024_l + 0.0061 HC02025_l + 0.0001 HC02026_l + 0.0518 HC02027_l + 0.0001 M01452_l + 0.0001 M01453_l + 0.0001 M01454_l + 0.0001 M01455_l + 0.0001 M01456_l + 0.0001 M01457_l + 0.0001 M01458_l + 0.0001 M01459_l + 0.0001 M01460_l + 0.0001 M01461_l + 0.0001 M01462_l + 0.0001 M01463_l + 0.0001 M01464_l + 0.0001 M01465_l + 0.0041 M01466_l + 0.0001 M01467_l + 0.0071 M01468_l + 0.0001 M01469_l + 0.0001 M01470_l + 0.0001 M01471_l + 0.0001 M01472_l + 0.0001 M01473_l + 0.0001 M01474_l + 0.0001 M01475_l + 0.0001 M01476_l + 0.0406 M01477_l + 0.0001 M01478_l + 0.0001 M01479_l + 0.0001 M01480_l + 0.0001 M01481_l + 0.0001 M01482_l + 0.0001 M01483_l + 0.0001 M01484_l + 0.0001 M01485_l + 0.0001 M01486_l + 0.0001 M01487_l + 0.005 M01490_l + 0.0001 M01491_l + 0.0001 M01492_l + 0.0001 M01494_l + 0.0001 M01495_l + 0.0001 M01496_l + 0.0001 M01497_l + 0.0001 M01498_l + 0.0081 M01501_l + 0.0001 M01502_l + 0.0001 M01506_l + 0.0001 M01508_l + 0.0001 M01509_l + 0.0001 M01510_l</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>[{'xolest_cho_l': 'C27H45RCO2'}, {'HC02020_l': 'C43H76O2'}, {'HC02021_l': 'C43H74O2'}, {'HC02022_l': 'C45H80O2'}, {'HC02023_l': 'C45H78O2'}, {'HC02024_l': 'C45H76O2'}, {'HC02025_l': 'C45H74O2'}, {'HC02026_l': 'C45H74O2'}, {'HC02027_l': 'C47H76O2'}, {'M01452_l': 'C49H80O2'}, {'M01453_l': 'C49H82O2'}, {'M01454_l': 'C44H76O2'}, {'M01455_l': 'C47H78O2'}, {'M01456_l': 'C47H80O2'}, {'M01457_l': 'C49H86O2'}, {'M01458_l': 'C47H82O2'}, {'M01459_l': 'C51H84O2'}, {'M01460_l': 'C49H82O2'}, {'M01461_l': 'C49H84O2'}, {'M01462_l': 'C49H86O2'}, {'M01463_l': 'C47H82O2'}, {'M01464_l': 'C45H78O2'}, {'M01465_l': 'C51H90O2'}, {'M01466_l': 'C49H76O2'}, {'M01467_l': 'C49H78O2'}, {'M01468_l': 'C47H74O2'}, {'M01469_l': 'C47H78O2'}, {'M01470_l': 'C41H70O2'}, {'M01471_l': 'C51H80O2'}, {'M01472_l': 'C51H82O2'}, {'M01473_l': 'C45H72O2'}, {'M01474_l': 'C45H76O2'}, {'M01475_l': 'C49H78O2'}, {'M01476_l': 'C49H80O2'}, {'M01477_l': 'C43H74O2'}, {'M01478_l': 'C45H78O2'}, {'M01479_l': 'C41H70O2'}, {'M01480_l': 'C47H76O2'}, {'M01481_l': 'C47H80O2'}, {'M01482_l': 'C51H82O2'}, {'M01483_l': 'C51H84O2'}, {'M01484_l': 'C47H82O2'}, {'M01485_l': 'C44H76O2'}, {'M01486_l': 'C45H78O2'}, {'M01487_l': 'C41H70O2'}, {'M01490_l': 'C47H78O2'}, {'M01491_l': 'C49H88O2'}, {'M01492_l': 'C47H84O2'}, {'M01494_l': 'C48H86O2'}, {'M01495_l': 'C44H78O2'}, {'M01496_l': 'C53H96O2'}, {'M01497_l': 'C53H94O2'}, {'M01498_l': 'C39H68O2'}, {'M01501_l': 'C41H72O2'}, {'M01502_l': 'C46H82O2'}, {'M01506_l': 'C42H74O2'}, {'M01508_l': 'C51H92O2'}, {'M01509_l': 'C50H90O2'}, {'M01510_l': 'C40H70O2'}]</t>
+        </is>
+      </c>
+      <c r="D756" t="inlineStr">
+        <is>
+          <t>{'C': 16.759499999999996, 'H': 31.326599999999992, 'R': -1, 'O': -0.00019999999999999963}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>